<commit_message>
Display of new tracks completed.
</commit_message>
<xml_diff>
--- a/macros123.xlsx
+++ b/macros123.xlsx
@@ -13,9 +13,10 @@
   </bookViews>
   <sheets>
     <sheet name="clump-related" sheetId="1" r:id="rId1"/>
-    <sheet name="single-cells" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="single-cells" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -489,14 +490,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1071,6 +1072,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
MACROS2 on macros123.xlsx now full
</commit_message>
<xml_diff>
--- a/macros123.xlsx
+++ b/macros123.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jsolisl\Documents\PhD\SW\macrosight\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsolisl/Documents/PhD/SW/macrosight/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C786A84-131C-5449-BA24-C68F59F5380D}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14685" yWindow="975" windowWidth="10005" windowHeight="12915"/>
+    <workbookView xWindow="9800" yWindow="980" windowWidth="14880" windowHeight="12920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clump-related" sheetId="1" r:id="rId1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="44">
   <si>
     <t>whichdataset</t>
   </si>
@@ -137,12 +138,33 @@
   </si>
   <si>
     <t>MACROS2-11</t>
+  </si>
+  <si>
+    <t>clumpinit</t>
+  </si>
+  <si>
+    <t>clumpfin</t>
+  </si>
+  <si>
+    <t>MACROS2-12</t>
+  </si>
+  <si>
+    <t>MACROS2-13</t>
+  </si>
+  <si>
+    <t>MACROS2-14</t>
+  </si>
+  <si>
+    <t>MACROS2-15</t>
+  </si>
+  <si>
+    <t>MACROS2-16</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -487,20 +509,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -516,8 +538,14 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -528,81 +556,111 @@
         <v>2</v>
       </c>
       <c r="D2">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E2">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="F2">
+        <v>34</v>
+      </c>
+      <c r="G2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>27</v>
       </c>
       <c r="B3">
-        <v>14002</v>
+        <v>3002</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D3">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="E3">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="F3">
+        <v>34</v>
+      </c>
+      <c r="G3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>28</v>
       </c>
       <c r="B4">
-        <v>19002</v>
+        <v>5004</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D4">
-        <v>290</v>
+        <v>4</v>
       </c>
       <c r="E4">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="F4">
+        <v>9</v>
+      </c>
+      <c r="G4">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>29</v>
       </c>
       <c r="B5">
-        <v>5004003</v>
+        <v>5004</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E5">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="F5">
+        <v>9</v>
+      </c>
+      <c r="G5">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>30</v>
       </c>
       <c r="B6">
-        <v>3002</v>
+        <v>6005</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D6">
-        <v>25</v>
+        <v>148</v>
       </c>
       <c r="E6">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+      <c r="F6">
+        <v>153</v>
+      </c>
+      <c r="G6">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -610,50 +668,68 @@
         <v>6005</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D7">
-        <v>133</v>
+        <v>148</v>
       </c>
       <c r="E7">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>224</v>
+      </c>
+      <c r="F7">
+        <v>153</v>
+      </c>
+      <c r="G7">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>32</v>
       </c>
       <c r="B8">
-        <v>6005004</v>
+        <v>6005</v>
       </c>
       <c r="C8">
         <v>5</v>
       </c>
       <c r="D8">
-        <v>170</v>
+        <v>221</v>
       </c>
       <c r="E8">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>291</v>
+      </c>
+      <c r="F8">
+        <v>225</v>
+      </c>
+      <c r="G8">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>33</v>
       </c>
       <c r="B9">
-        <v>8007</v>
+        <v>6005</v>
       </c>
       <c r="C9">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D9">
-        <v>29</v>
+        <v>221</v>
       </c>
       <c r="E9">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>291</v>
+      </c>
+      <c r="F9">
+        <v>225</v>
+      </c>
+      <c r="G9">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -661,403 +737,536 @@
         <v>8007</v>
       </c>
       <c r="C10">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D10">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E10">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="F10">
+        <v>24</v>
+      </c>
+      <c r="G10">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>35</v>
       </c>
       <c r="B11">
-        <v>8006004</v>
+        <v>8007</v>
       </c>
       <c r="C11">
         <v>8</v>
       </c>
       <c r="D11">
-        <v>170</v>
+        <v>19</v>
       </c>
       <c r="E11">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="F11">
+        <v>24</v>
+      </c>
+      <c r="G11">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>36</v>
       </c>
       <c r="B12">
+        <v>8007</v>
+      </c>
+      <c r="C12">
+        <v>7</v>
+      </c>
+      <c r="D12">
+        <v>39</v>
+      </c>
+      <c r="E12">
+        <v>53</v>
+      </c>
+      <c r="F12">
+        <v>44</v>
+      </c>
+      <c r="G12">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13">
+        <v>8007</v>
+      </c>
+      <c r="C13">
+        <v>8</v>
+      </c>
+      <c r="D13">
+        <v>39</v>
+      </c>
+      <c r="E13">
+        <v>53</v>
+      </c>
+      <c r="F13">
+        <v>44</v>
+      </c>
+      <c r="G13">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14">
         <v>19002</v>
       </c>
-      <c r="C12">
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>305</v>
+      </c>
+      <c r="E14">
+        <v>315</v>
+      </c>
+      <c r="F14">
+        <v>310</v>
+      </c>
+      <c r="G14">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15">
+        <v>19002</v>
+      </c>
+      <c r="C15">
         <v>19</v>
       </c>
-      <c r="D12">
-        <v>290</v>
-      </c>
-      <c r="E12">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13">
-        <v>2001</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <v>147</v>
-      </c>
-      <c r="E13">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14">
-        <v>22001</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14">
-        <v>385</v>
-      </c>
-      <c r="E14">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15">
-        <v>29001</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
       <c r="D15">
-        <v>385</v>
+        <v>305</v>
       </c>
       <c r="E15">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>315</v>
+      </c>
+      <c r="F15">
+        <v>310</v>
+      </c>
+      <c r="G15">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="B16">
-        <v>2001</v>
+        <v>19002</v>
       </c>
       <c r="C16">
         <v>2</v>
       </c>
       <c r="D16">
+        <v>337</v>
+      </c>
+      <c r="E16">
+        <v>345</v>
+      </c>
+      <c r="F16">
+        <v>342</v>
+      </c>
+      <c r="G16">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17">
+        <v>19002</v>
+      </c>
+      <c r="C17">
+        <v>19</v>
+      </c>
+      <c r="D17">
+        <v>337</v>
+      </c>
+      <c r="E17">
+        <v>345</v>
+      </c>
+      <c r="F17">
+        <v>342</v>
+      </c>
+      <c r="G17">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <v>2001</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
         <v>147</v>
       </c>
-      <c r="E16">
+      <c r="E18">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19">
+        <v>22001</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>385</v>
+      </c>
+      <c r="E19">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20">
+        <v>29001</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>385</v>
+      </c>
+      <c r="E20">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21">
+        <v>2001</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>147</v>
+      </c>
+      <c r="E21">
         <v>190</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>9</v>
       </c>
-      <c r="B17">
+      <c r="B22">
         <v>3002</v>
       </c>
-      <c r="C17">
+      <c r="C22">
         <v>2</v>
       </c>
-      <c r="D17">
+      <c r="D22">
         <v>200</v>
       </c>
-      <c r="E17">
+      <c r="E22">
         <v>280</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>10</v>
       </c>
-      <c r="B18">
+      <c r="B23">
         <v>3002</v>
       </c>
-      <c r="C18">
+      <c r="C23">
         <v>3</v>
       </c>
-      <c r="D18">
+      <c r="D23">
         <v>200</v>
       </c>
-      <c r="E18">
+      <c r="E23">
         <v>280</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>11</v>
       </c>
-      <c r="B19">
+      <c r="B24">
         <v>3002</v>
       </c>
-      <c r="C19">
+      <c r="C24">
         <v>3</v>
       </c>
-      <c r="D19">
+      <c r="D24">
         <v>361</v>
       </c>
-      <c r="E19">
+      <c r="E24">
         <v>393</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>12</v>
       </c>
-      <c r="B20">
+      <c r="B25">
         <v>9005003</v>
       </c>
-      <c r="C20">
+      <c r="C25">
         <v>5</v>
       </c>
-      <c r="D20">
+      <c r="D25">
         <v>17</v>
       </c>
-      <c r="E20">
+      <c r="E25">
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>13</v>
       </c>
-      <c r="B21">
+      <c r="B26">
         <v>5004003002</v>
       </c>
-      <c r="C21">
+      <c r="C26">
         <v>5</v>
       </c>
-      <c r="D21">
+      <c r="D26">
         <v>66</v>
       </c>
-      <c r="E21">
+      <c r="E26">
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>14</v>
       </c>
-      <c r="B22">
+      <c r="B27">
         <v>17005</v>
       </c>
-      <c r="C22">
+      <c r="C27">
         <v>5</v>
       </c>
-      <c r="D22">
+      <c r="D27">
         <v>76</v>
       </c>
-      <c r="E22">
+      <c r="E27">
         <v>110</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>15</v>
       </c>
-      <c r="B23">
+      <c r="B28">
         <v>9006</v>
       </c>
-      <c r="C23">
+      <c r="C28">
         <v>6</v>
       </c>
-      <c r="D23">
+      <c r="D28">
         <v>42</v>
       </c>
-      <c r="E23">
+      <c r="E28">
         <v>76</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>16</v>
       </c>
-      <c r="B24">
+      <c r="B29">
         <v>19008</v>
       </c>
-      <c r="C24">
+      <c r="C29">
         <v>8</v>
       </c>
-      <c r="D24">
+      <c r="D29">
         <v>108</v>
       </c>
-      <c r="E24">
+      <c r="E29">
         <v>131</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>17</v>
       </c>
-      <c r="B25">
+      <c r="B30">
         <v>19008</v>
       </c>
-      <c r="C25">
+      <c r="C30">
         <v>8</v>
       </c>
-      <c r="D25">
+      <c r="D30">
         <v>125</v>
       </c>
-      <c r="E25">
+      <c r="E30">
         <v>140</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>18</v>
       </c>
-      <c r="B26">
+      <c r="B31">
         <v>9005004003002</v>
       </c>
-      <c r="C26">
+      <c r="C31">
         <v>9</v>
       </c>
-      <c r="D26">
+      <c r="D31">
         <v>36</v>
       </c>
-      <c r="E26">
+      <c r="E31">
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>19</v>
       </c>
-      <c r="B27">
+      <c r="B32">
         <v>9006</v>
       </c>
-      <c r="C27">
+      <c r="C32">
         <v>9</v>
       </c>
-      <c r="D27">
+      <c r="D32">
         <v>48</v>
       </c>
-      <c r="E27">
+      <c r="E32">
         <v>75</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>20</v>
       </c>
-      <c r="B28">
+      <c r="B33">
         <v>9003002</v>
       </c>
-      <c r="C28">
+      <c r="C33">
         <v>9</v>
       </c>
-      <c r="D28">
+      <c r="D33">
         <v>86</v>
       </c>
-      <c r="E28">
+      <c r="E33">
         <v>105</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>21</v>
       </c>
-      <c r="B29">
+      <c r="B34">
         <v>11005</v>
       </c>
-      <c r="C29">
+      <c r="C34">
         <v>11</v>
       </c>
-      <c r="D29">
+      <c r="D34">
         <v>35</v>
       </c>
-      <c r="E29">
+      <c r="E34">
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>22</v>
       </c>
-      <c r="B30">
+      <c r="B35">
         <v>17005</v>
       </c>
-      <c r="C30">
+      <c r="C35">
         <v>17</v>
       </c>
-      <c r="D30">
+      <c r="D35">
         <v>79</v>
       </c>
-      <c r="E30">
+      <c r="E35">
         <v>105</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>23</v>
       </c>
-      <c r="B31">
+      <c r="B36">
         <v>19008</v>
       </c>
-      <c r="C31">
+      <c r="C36">
         <v>19</v>
       </c>
-      <c r="D31">
+      <c r="D36">
         <v>108</v>
       </c>
-      <c r="E31">
+      <c r="E36">
         <v>131</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>24</v>
       </c>
-      <c r="B32">
+      <c r="B37">
         <v>19008</v>
       </c>
-      <c r="C32">
+      <c r="C37">
         <v>19</v>
       </c>
-      <c r="D32">
+      <c r="D37">
         <v>125</v>
       </c>
-      <c r="E32">
+      <c r="E37">
         <v>140</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>25</v>
       </c>
-      <c r="B33">
+      <c r="B38">
         <v>22001</v>
       </c>
-      <c r="C33">
+      <c r="C38">
         <v>22</v>
       </c>
-      <c r="D33">
+      <c r="D38">
         <v>385</v>
       </c>
-      <c r="E33">
+      <c r="E38">
         <v>409</v>
       </c>
     </row>
@@ -1067,24 +1276,244 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="101" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:G1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19">
+        <v>3002</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>25</v>
+      </c>
+      <c r="E19">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20">
+        <v>14002</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>49</v>
+      </c>
+      <c r="E20">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21">
+        <v>19002</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>290</v>
+      </c>
+      <c r="E21">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22">
+        <v>5004003</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="E22">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23">
+        <v>3002</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23">
+        <v>25</v>
+      </c>
+      <c r="E23">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24">
+        <v>6005</v>
+      </c>
+      <c r="C24">
+        <v>5</v>
+      </c>
+      <c r="D24">
+        <v>133</v>
+      </c>
+      <c r="E24">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25">
+        <v>6005004</v>
+      </c>
+      <c r="C25">
+        <v>5</v>
+      </c>
+      <c r="D25">
+        <v>170</v>
+      </c>
+      <c r="E25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26">
+        <v>8007</v>
+      </c>
+      <c r="C26">
+        <v>7</v>
+      </c>
+      <c r="D26">
+        <v>29</v>
+      </c>
+      <c r="E26">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27">
+        <v>8007</v>
+      </c>
+      <c r="C27">
+        <v>8</v>
+      </c>
+      <c r="D27">
+        <v>29</v>
+      </c>
+      <c r="E27">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28">
+        <v>8006004</v>
+      </c>
+      <c r="C28">
+        <v>8</v>
+      </c>
+      <c r="D28">
+        <v>170</v>
+      </c>
+      <c r="E28">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29">
+        <v>19002</v>
+      </c>
+      <c r="C29">
+        <v>19</v>
+      </c>
+      <c r="D29">
+        <v>290</v>
+      </c>
+      <c r="E29">
+        <v>330</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
various: macrossingles123, initscript, reviewdatasets
</commit_message>
<xml_diff>
--- a/macros123.xlsx
+++ b/macros123.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jsolisl\Documents\PhD\SW\macrosight\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsolislemus/Documents/PhD/SW/macrosight/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6658A9C6-D809-144C-A62A-8E0177A7287E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9795" yWindow="975" windowWidth="14880" windowHeight="12915"/>
+    <workbookView xWindow="6460" yWindow="460" windowWidth="26080" windowHeight="19920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clump-related" sheetId="1" r:id="rId1"/>
     <sheet name="single-cells" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="115">
   <si>
     <t>whichdataset</t>
   </si>
@@ -239,13 +240,145 @@
   </si>
   <si>
     <t>macros3-20</t>
+  </si>
+  <si>
+    <t>macros1-1</t>
+  </si>
+  <si>
+    <t>macros1-2</t>
+  </si>
+  <si>
+    <t>macros1-3</t>
+  </si>
+  <si>
+    <t>macros1-4</t>
+  </si>
+  <si>
+    <t>macros1-5</t>
+  </si>
+  <si>
+    <t>macros1-6</t>
+  </si>
+  <si>
+    <t>macros1-7</t>
+  </si>
+  <si>
+    <t>macros1-8</t>
+  </si>
+  <si>
+    <t>macros1-9</t>
+  </si>
+  <si>
+    <t>macros1-10</t>
+  </si>
+  <si>
+    <t>macros1-11</t>
+  </si>
+  <si>
+    <t>macros1-12</t>
+  </si>
+  <si>
+    <t>macros1-13</t>
+  </si>
+  <si>
+    <t>macros1-14</t>
+  </si>
+  <si>
+    <t>macros1-15</t>
+  </si>
+  <si>
+    <t>macros1-16</t>
+  </si>
+  <si>
+    <t>macros1-17</t>
+  </si>
+  <si>
+    <t>macros1-18</t>
+  </si>
+  <si>
+    <t>macros1-19</t>
+  </si>
+  <si>
+    <t>macros1-20</t>
+  </si>
+  <si>
+    <t>macros1-21</t>
+  </si>
+  <si>
+    <t>macros1-22</t>
+  </si>
+  <si>
+    <t>macros1-23</t>
+  </si>
+  <si>
+    <t>macros1-24</t>
+  </si>
+  <si>
+    <t>macros1-25</t>
+  </si>
+  <si>
+    <t>macros1-26</t>
+  </si>
+  <si>
+    <t>macros1-27</t>
+  </si>
+  <si>
+    <t>macros1-28</t>
+  </si>
+  <si>
+    <t>macros1-29</t>
+  </si>
+  <si>
+    <t>macros1-30</t>
+  </si>
+  <si>
+    <t>macros1-31</t>
+  </si>
+  <si>
+    <t>macros1-32</t>
+  </si>
+  <si>
+    <t>macros1-33</t>
+  </si>
+  <si>
+    <t>macros1-34</t>
+  </si>
+  <si>
+    <t>macros1-35</t>
+  </si>
+  <si>
+    <t>macros1-36</t>
+  </si>
+  <si>
+    <t>macros1-37</t>
+  </si>
+  <si>
+    <t>macros1-38</t>
+  </si>
+  <si>
+    <t>macros1-39</t>
+  </si>
+  <si>
+    <t>macros1-40</t>
+  </si>
+  <si>
+    <t>macros1-41</t>
+  </si>
+  <si>
+    <t>macros1-42</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -253,8 +386,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -276,6 +424,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -409,7 +563,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -433,11 +587,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -746,25 +928,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H38"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K77" sqref="K77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -787,7 +969,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>26</v>
       </c>
@@ -810,7 +992,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>27</v>
       </c>
@@ -833,7 +1015,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>28</v>
       </c>
@@ -856,7 +1038,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>29</v>
       </c>
@@ -879,7 +1061,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>30</v>
       </c>
@@ -902,7 +1084,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>31</v>
       </c>
@@ -925,7 +1107,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>32</v>
       </c>
@@ -948,7 +1130,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>33</v>
       </c>
@@ -971,7 +1153,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>34</v>
       </c>
@@ -994,7 +1176,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>35</v>
       </c>
@@ -1017,7 +1199,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>36</v>
       </c>
@@ -1040,7 +1222,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>39</v>
       </c>
@@ -1063,7 +1245,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>40</v>
       </c>
@@ -1086,7 +1268,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>41</v>
       </c>
@@ -1109,7 +1291,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>42</v>
       </c>
@@ -1132,7 +1314,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>43</v>
       </c>
@@ -1155,7 +1337,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>48</v>
       </c>
@@ -1178,7 +1360,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>51</v>
       </c>
@@ -1201,7 +1383,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>52</v>
       </c>
@@ -1224,7 +1406,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>53</v>
       </c>
@@ -1247,7 +1429,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>54</v>
       </c>
@@ -1270,7 +1452,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>55</v>
       </c>
@@ -1293,7 +1475,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>56</v>
       </c>
@@ -1316,7 +1498,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
         <v>57</v>
       </c>
@@ -1339,7 +1521,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
         <v>58</v>
       </c>
@@ -1362,7 +1544,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
         <v>59</v>
       </c>
@@ -1385,7 +1567,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
         <v>60</v>
       </c>
@@ -1408,7 +1590,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
         <v>61</v>
       </c>
@@ -1431,7 +1613,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
         <v>62</v>
       </c>
@@ -1454,7 +1636,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
         <v>63</v>
       </c>
@@ -1477,7 +1659,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
         <v>64</v>
       </c>
@@ -1500,7 +1682,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
         <v>65</v>
       </c>
@@ -1523,7 +1705,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
         <v>66</v>
       </c>
@@ -1546,7 +1728,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
         <v>67</v>
       </c>
@@ -1569,7 +1751,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
         <v>68</v>
       </c>
@@ -1591,8 +1773,16 @@
       <c r="G36" s="21">
         <v>233</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I36" s="24"/>
+      <c r="J36" s="24"/>
+      <c r="K36" s="24"/>
+      <c r="L36" s="24"/>
+      <c r="M36" s="24"/>
+      <c r="N36" s="24"/>
+      <c r="O36" s="24"/>
+      <c r="P36" s="24"/>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
         <v>69</v>
       </c>
@@ -1614,8 +1804,16 @@
       <c r="G37" s="21">
         <v>45</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I37" s="24"/>
+      <c r="J37" s="24"/>
+      <c r="K37" s="24"/>
+      <c r="L37" s="24"/>
+      <c r="M37" s="24"/>
+      <c r="N37" s="24"/>
+      <c r="O37" s="24"/>
+      <c r="P37" s="24"/>
+    </row>
+    <row r="38" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>70</v>
       </c>
@@ -1637,34 +1835,1344 @@
       <c r="G38" s="22">
         <v>402</v>
       </c>
+      <c r="I38" s="24"/>
+      <c r="J38" s="24"/>
+      <c r="K38" s="24"/>
+      <c r="L38" s="24"/>
+      <c r="M38" s="24"/>
+      <c r="N38" s="24"/>
+      <c r="O38" s="24"/>
+      <c r="P38" s="24"/>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A39" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="B39" s="24">
+        <v>8002</v>
+      </c>
+      <c r="C39" s="24">
+        <v>2</v>
+      </c>
+      <c r="D39" s="24">
+        <v>248</v>
+      </c>
+      <c r="E39" s="24">
+        <v>258</v>
+      </c>
+      <c r="F39" s="24">
+        <v>251</v>
+      </c>
+      <c r="G39" s="25">
+        <v>255</v>
+      </c>
+      <c r="H39" t="s">
+        <v>114</v>
+      </c>
+      <c r="I39" s="24"/>
+      <c r="J39" s="24"/>
+      <c r="K39" s="24"/>
+      <c r="L39" s="24"/>
+      <c r="M39" s="24"/>
+      <c r="N39" s="24"/>
+      <c r="O39" s="24"/>
+      <c r="P39" s="24"/>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A40" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="B40" s="26">
+        <v>8002</v>
+      </c>
+      <c r="C40" s="26">
+        <v>8</v>
+      </c>
+      <c r="D40" s="26">
+        <v>246</v>
+      </c>
+      <c r="E40" s="26">
+        <v>258</v>
+      </c>
+      <c r="F40" s="26">
+        <v>251</v>
+      </c>
+      <c r="G40" s="27">
+        <v>255</v>
+      </c>
+      <c r="H40" t="s">
+        <v>114</v>
+      </c>
+      <c r="I40" s="24"/>
+      <c r="J40" s="24"/>
+      <c r="K40" s="24"/>
+      <c r="L40" s="24"/>
+      <c r="M40" s="24"/>
+      <c r="N40" s="24"/>
+      <c r="O40" s="24"/>
+      <c r="P40" s="24"/>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A41" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="B41" s="24">
+        <v>8002</v>
+      </c>
+      <c r="C41" s="24">
+        <v>2</v>
+      </c>
+      <c r="D41" s="24">
+        <v>412</v>
+      </c>
+      <c r="E41" s="24">
+        <v>422</v>
+      </c>
+      <c r="F41" s="24">
+        <v>417</v>
+      </c>
+      <c r="G41" s="25">
+        <v>417</v>
+      </c>
+      <c r="H41" t="s">
+        <v>113</v>
+      </c>
+      <c r="I41" s="24"/>
+      <c r="J41" s="24"/>
+      <c r="K41" s="24"/>
+      <c r="L41" s="24"/>
+      <c r="M41" s="24"/>
+      <c r="N41" s="24"/>
+      <c r="O41" s="24"/>
+      <c r="P41" s="24"/>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A42" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="B42" s="24">
+        <v>8002</v>
+      </c>
+      <c r="C42" s="24">
+        <v>8</v>
+      </c>
+      <c r="D42" s="24">
+        <v>412</v>
+      </c>
+      <c r="E42" s="24">
+        <v>422</v>
+      </c>
+      <c r="F42" s="24">
+        <v>417</v>
+      </c>
+      <c r="G42" s="25">
+        <v>417</v>
+      </c>
+      <c r="H42" t="s">
+        <v>113</v>
+      </c>
+      <c r="I42" s="24"/>
+      <c r="J42" s="24"/>
+      <c r="K42" s="24"/>
+      <c r="L42" s="24"/>
+      <c r="M42" s="24"/>
+      <c r="N42" s="24"/>
+      <c r="O42" s="24"/>
+      <c r="P42" s="24"/>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A43" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="B43" s="24">
+        <v>8007</v>
+      </c>
+      <c r="C43" s="24">
+        <v>7</v>
+      </c>
+      <c r="D43" s="24">
+        <v>175</v>
+      </c>
+      <c r="E43" s="24">
+        <v>188</v>
+      </c>
+      <c r="F43" s="24">
+        <v>181</v>
+      </c>
+      <c r="G43" s="25">
+        <v>184</v>
+      </c>
+      <c r="H43" t="s">
+        <v>114</v>
+      </c>
+      <c r="I43" s="24"/>
+      <c r="J43" s="24"/>
+      <c r="K43" s="24"/>
+      <c r="L43" s="24"/>
+      <c r="M43" s="24"/>
+      <c r="N43" s="24"/>
+      <c r="O43" s="24"/>
+      <c r="P43" s="24"/>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A44" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="B44" s="24">
+        <v>8007</v>
+      </c>
+      <c r="C44" s="24">
+        <v>8</v>
+      </c>
+      <c r="D44" s="24">
+        <v>175</v>
+      </c>
+      <c r="E44" s="24">
+        <v>188</v>
+      </c>
+      <c r="F44" s="24">
+        <v>181</v>
+      </c>
+      <c r="G44" s="25">
+        <v>184</v>
+      </c>
+      <c r="H44" t="s">
+        <v>114</v>
+      </c>
+      <c r="I44" s="24"/>
+      <c r="J44" s="24"/>
+      <c r="K44" s="24"/>
+      <c r="L44" s="24"/>
+      <c r="M44" s="24"/>
+      <c r="N44" s="24"/>
+      <c r="O44" s="24"/>
+      <c r="P44" s="24"/>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A45" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="B45" s="24">
+        <v>11010</v>
+      </c>
+      <c r="C45">
+        <v>10</v>
+      </c>
+      <c r="D45" s="24">
+        <v>1</v>
+      </c>
+      <c r="E45" s="24">
+        <v>140</v>
+      </c>
+      <c r="F45" s="24">
+        <v>2</v>
+      </c>
+      <c r="G45" s="25">
+        <v>135</v>
+      </c>
+      <c r="H45" t="s">
+        <v>114</v>
+      </c>
+      <c r="I45" s="24"/>
+      <c r="J45" s="24"/>
+      <c r="K45" s="24"/>
+      <c r="L45" s="24"/>
+      <c r="M45" s="24"/>
+      <c r="N45" s="24"/>
+      <c r="O45" s="24"/>
+      <c r="P45" s="24"/>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A46" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="B46" s="24">
+        <v>11010</v>
+      </c>
+      <c r="C46">
+        <v>11</v>
+      </c>
+      <c r="D46" s="24">
+        <v>1</v>
+      </c>
+      <c r="E46" s="24">
+        <v>140</v>
+      </c>
+      <c r="F46" s="24">
+        <v>2</v>
+      </c>
+      <c r="G46" s="25">
+        <v>135</v>
+      </c>
+      <c r="H46" t="s">
+        <v>114</v>
+      </c>
+      <c r="I46" s="24"/>
+      <c r="J46" s="24"/>
+      <c r="K46" s="24"/>
+      <c r="L46" s="24"/>
+      <c r="M46" s="24"/>
+      <c r="N46" s="24"/>
+      <c r="O46" s="24"/>
+      <c r="P46" s="24"/>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A47" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="B47" s="24">
+        <v>14013</v>
+      </c>
+      <c r="C47">
+        <v>13</v>
+      </c>
+      <c r="D47" s="24">
+        <v>294</v>
+      </c>
+      <c r="E47" s="24">
+        <v>368</v>
+      </c>
+      <c r="F47" s="24">
+        <v>299</v>
+      </c>
+      <c r="G47" s="25">
+        <v>263</v>
+      </c>
+      <c r="H47" t="s">
+        <v>114</v>
+      </c>
+      <c r="I47" s="24"/>
+      <c r="J47" s="24"/>
+      <c r="K47" s="24"/>
+      <c r="L47" s="24"/>
+      <c r="M47" s="24"/>
+      <c r="N47" s="24"/>
+      <c r="O47" s="24"/>
+      <c r="P47" s="24"/>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A48" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="B48" s="24">
+        <v>14013</v>
+      </c>
+      <c r="C48">
+        <v>14</v>
+      </c>
+      <c r="D48" s="24">
+        <v>294</v>
+      </c>
+      <c r="E48" s="24">
+        <v>368</v>
+      </c>
+      <c r="F48" s="24">
+        <v>299</v>
+      </c>
+      <c r="G48" s="25">
+        <v>263</v>
+      </c>
+      <c r="H48" t="s">
+        <v>114</v>
+      </c>
+      <c r="I48" s="24"/>
+      <c r="J48" s="24"/>
+      <c r="K48" s="24"/>
+      <c r="L48" s="24"/>
+      <c r="M48" s="24"/>
+      <c r="N48" s="24"/>
+      <c r="O48" s="24"/>
+      <c r="P48" s="24"/>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A49" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="B49" s="24">
+        <v>16012</v>
+      </c>
+      <c r="C49">
+        <v>12</v>
+      </c>
+      <c r="D49" s="24">
+        <v>15</v>
+      </c>
+      <c r="E49" s="24">
+        <v>35</v>
+      </c>
+      <c r="F49" s="24">
+        <v>20</v>
+      </c>
+      <c r="G49" s="25">
+        <v>30</v>
+      </c>
+      <c r="H49" t="s">
+        <v>114</v>
+      </c>
+      <c r="I49" s="24"/>
+      <c r="J49" s="24"/>
+      <c r="K49" s="24"/>
+      <c r="L49" s="24"/>
+      <c r="M49" s="24"/>
+      <c r="N49" s="24"/>
+      <c r="O49" s="24"/>
+      <c r="P49" s="24"/>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A50" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="B50" s="24">
+        <v>16012</v>
+      </c>
+      <c r="C50">
+        <v>16</v>
+      </c>
+      <c r="D50" s="24">
+        <v>15</v>
+      </c>
+      <c r="E50" s="24">
+        <v>35</v>
+      </c>
+      <c r="F50" s="24">
+        <v>20</v>
+      </c>
+      <c r="G50" s="25">
+        <v>30</v>
+      </c>
+      <c r="H50" t="s">
+        <v>114</v>
+      </c>
+      <c r="I50" s="24"/>
+      <c r="J50" s="24"/>
+      <c r="K50" s="24"/>
+      <c r="L50" s="24"/>
+      <c r="M50" s="24"/>
+      <c r="N50" s="24"/>
+      <c r="O50" s="24"/>
+      <c r="P50" s="24"/>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A51" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="B51" s="24">
+        <v>19002</v>
+      </c>
+      <c r="C51">
+        <v>2</v>
+      </c>
+      <c r="D51" s="24">
+        <v>78</v>
+      </c>
+      <c r="E51" s="24">
+        <v>96</v>
+      </c>
+      <c r="F51" s="24">
+        <v>83</v>
+      </c>
+      <c r="G51" s="25">
+        <v>91</v>
+      </c>
+      <c r="H51" t="s">
+        <v>114</v>
+      </c>
+      <c r="I51" s="24"/>
+      <c r="J51" s="24"/>
+      <c r="K51" s="24"/>
+      <c r="L51" s="24"/>
+      <c r="M51" s="24"/>
+      <c r="N51" s="24"/>
+      <c r="O51" s="24"/>
+      <c r="P51" s="24"/>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A52" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="B52" s="26">
+        <v>19002</v>
+      </c>
+      <c r="C52" s="26">
+        <v>19</v>
+      </c>
+      <c r="D52" s="26">
+        <v>78</v>
+      </c>
+      <c r="E52" s="26">
+        <v>96</v>
+      </c>
+      <c r="F52" s="26">
+        <v>83</v>
+      </c>
+      <c r="G52" s="27">
+        <v>91</v>
+      </c>
+      <c r="H52" t="s">
+        <v>114</v>
+      </c>
+      <c r="I52" s="24"/>
+      <c r="J52" s="24"/>
+      <c r="K52" s="24"/>
+      <c r="L52" s="24"/>
+      <c r="M52" s="24"/>
+      <c r="N52" s="24"/>
+      <c r="O52" s="24"/>
+      <c r="P52" s="24"/>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A53" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="B53" s="24">
+        <v>20001</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53" s="24">
+        <v>108</v>
+      </c>
+      <c r="E53" s="24">
+        <v>126</v>
+      </c>
+      <c r="F53" s="24">
+        <v>113</v>
+      </c>
+      <c r="G53" s="25">
+        <v>121</v>
+      </c>
+      <c r="H53" t="s">
+        <v>113</v>
+      </c>
+      <c r="I53" s="24"/>
+      <c r="J53" s="24"/>
+      <c r="K53" s="24"/>
+      <c r="L53" s="24"/>
+      <c r="M53" s="24"/>
+      <c r="N53" s="24"/>
+      <c r="O53" s="24"/>
+      <c r="P53" s="24"/>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A54" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="B54" s="24">
+        <v>20001</v>
+      </c>
+      <c r="C54">
+        <v>20</v>
+      </c>
+      <c r="D54" s="24">
+        <v>108</v>
+      </c>
+      <c r="E54" s="24">
+        <v>126</v>
+      </c>
+      <c r="F54" s="24">
+        <v>113</v>
+      </c>
+      <c r="G54" s="25">
+        <v>121</v>
+      </c>
+      <c r="H54" t="s">
+        <v>113</v>
+      </c>
+      <c r="I54" s="24"/>
+      <c r="J54" s="24"/>
+      <c r="K54" s="24"/>
+      <c r="L54" s="24"/>
+      <c r="M54" s="24"/>
+      <c r="N54" s="24"/>
+      <c r="O54" s="24"/>
+      <c r="P54" s="24"/>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A55" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="B55" s="24">
+        <v>20005</v>
+      </c>
+      <c r="C55">
+        <v>5</v>
+      </c>
+      <c r="D55" s="24">
+        <v>66</v>
+      </c>
+      <c r="E55" s="24">
+        <v>91</v>
+      </c>
+      <c r="F55" s="24">
+        <v>71</v>
+      </c>
+      <c r="G55" s="25">
+        <v>85</v>
+      </c>
+      <c r="H55" t="s">
+        <v>114</v>
+      </c>
+      <c r="I55" s="24"/>
+      <c r="J55" s="24"/>
+      <c r="K55" s="24"/>
+      <c r="L55" s="24"/>
+      <c r="M55" s="24"/>
+      <c r="N55" s="24"/>
+      <c r="O55" s="24"/>
+      <c r="P55" s="24"/>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A56" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="B56" s="24">
+        <v>20005</v>
+      </c>
+      <c r="C56">
+        <v>20</v>
+      </c>
+      <c r="D56" s="24">
+        <v>66</v>
+      </c>
+      <c r="E56" s="24">
+        <v>91</v>
+      </c>
+      <c r="F56" s="24">
+        <v>71</v>
+      </c>
+      <c r="G56" s="25">
+        <v>86</v>
+      </c>
+      <c r="H56" t="s">
+        <v>114</v>
+      </c>
+      <c r="I56" s="24"/>
+      <c r="J56" s="24"/>
+      <c r="K56" s="24"/>
+      <c r="L56" s="24"/>
+      <c r="M56" s="24"/>
+      <c r="N56" s="24"/>
+      <c r="O56" s="24"/>
+      <c r="P56" s="24"/>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A57" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="B57" s="24">
+        <v>20005</v>
+      </c>
+      <c r="C57">
+        <v>5</v>
+      </c>
+      <c r="D57" s="24">
+        <v>94</v>
+      </c>
+      <c r="E57" s="24">
+        <v>104</v>
+      </c>
+      <c r="F57" s="24">
+        <v>99</v>
+      </c>
+      <c r="G57" s="25">
+        <v>99</v>
+      </c>
+      <c r="H57" t="s">
+        <v>113</v>
+      </c>
+      <c r="I57" s="24"/>
+      <c r="J57" s="24"/>
+      <c r="K57" s="24"/>
+      <c r="L57" s="24"/>
+      <c r="M57" s="24"/>
+      <c r="N57" s="24"/>
+      <c r="O57" s="24"/>
+      <c r="P57" s="24"/>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A58" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="B58" s="24">
+        <v>20005</v>
+      </c>
+      <c r="C58">
+        <v>20</v>
+      </c>
+      <c r="D58" s="24">
+        <v>94</v>
+      </c>
+      <c r="E58" s="24">
+        <v>104</v>
+      </c>
+      <c r="F58" s="24">
+        <v>99</v>
+      </c>
+      <c r="G58" s="25">
+        <v>99</v>
+      </c>
+      <c r="H58" t="s">
+        <v>113</v>
+      </c>
+      <c r="I58" s="24"/>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A59" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="B59" s="24">
+        <v>23020</v>
+      </c>
+      <c r="C59">
+        <v>20</v>
+      </c>
+      <c r="D59" s="24">
+        <v>31</v>
+      </c>
+      <c r="E59" s="24">
+        <v>49</v>
+      </c>
+      <c r="F59" s="24">
+        <v>36</v>
+      </c>
+      <c r="G59" s="25">
+        <v>44</v>
+      </c>
+      <c r="H59" t="s">
+        <v>114</v>
+      </c>
+      <c r="I59" s="24"/>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A60" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="B60" s="24">
+        <v>23020</v>
+      </c>
+      <c r="C60">
+        <v>23</v>
+      </c>
+      <c r="D60" s="24">
+        <v>31</v>
+      </c>
+      <c r="E60" s="24">
+        <v>49</v>
+      </c>
+      <c r="F60" s="24">
+        <v>36</v>
+      </c>
+      <c r="G60" s="25">
+        <v>44</v>
+      </c>
+      <c r="H60" t="s">
+        <v>114</v>
+      </c>
+      <c r="I60" s="24"/>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A61" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="B61" s="24">
+        <v>42038</v>
+      </c>
+      <c r="C61">
+        <v>38</v>
+      </c>
+      <c r="D61" s="24">
+        <v>122</v>
+      </c>
+      <c r="E61" s="24">
+        <v>134</v>
+      </c>
+      <c r="F61" s="24">
+        <v>126</v>
+      </c>
+      <c r="G61" s="25">
+        <v>129</v>
+      </c>
+      <c r="H61" t="s">
+        <v>114</v>
+      </c>
+      <c r="I61" s="24"/>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A62" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="B62" s="24">
+        <v>46010</v>
+      </c>
+      <c r="C62">
+        <v>10</v>
+      </c>
+      <c r="D62" s="24">
+        <v>139</v>
+      </c>
+      <c r="E62" s="24">
+        <v>151</v>
+      </c>
+      <c r="F62" s="24">
+        <v>144</v>
+      </c>
+      <c r="G62" s="25">
+        <v>146</v>
+      </c>
+      <c r="H62" t="s">
+        <v>114</v>
+      </c>
+      <c r="I62" s="24"/>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A63" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="B63" s="24">
+        <v>47043</v>
+      </c>
+      <c r="C63">
+        <v>43</v>
+      </c>
+      <c r="D63" s="24">
+        <v>147</v>
+      </c>
+      <c r="E63" s="24">
+        <v>158</v>
+      </c>
+      <c r="F63" s="24">
+        <v>151</v>
+      </c>
+      <c r="G63" s="25">
+        <v>153</v>
+      </c>
+      <c r="H63" t="s">
+        <v>114</v>
+      </c>
+      <c r="I63" s="24"/>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A64" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="B64" s="24">
+        <v>50002</v>
+      </c>
+      <c r="C64">
+        <v>2</v>
+      </c>
+      <c r="D64" s="24">
+        <v>171</v>
+      </c>
+      <c r="E64" s="24">
+        <v>183</v>
+      </c>
+      <c r="F64" s="24">
+        <v>176</v>
+      </c>
+      <c r="G64" s="25">
+        <v>178</v>
+      </c>
+      <c r="H64" t="s">
+        <v>113</v>
+      </c>
+      <c r="I64" s="24"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A65" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="B65" s="24">
+        <v>50002</v>
+      </c>
+      <c r="C65">
+        <v>50</v>
+      </c>
+      <c r="D65" s="24">
+        <v>171</v>
+      </c>
+      <c r="E65" s="24">
+        <v>183</v>
+      </c>
+      <c r="F65" s="24">
+        <v>176</v>
+      </c>
+      <c r="G65" s="25">
+        <v>178</v>
+      </c>
+      <c r="H65" t="s">
+        <v>113</v>
+      </c>
+      <c r="I65" s="24"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A66" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="B66" s="24">
+        <v>60002</v>
+      </c>
+      <c r="C66">
+        <v>2</v>
+      </c>
+      <c r="D66" s="24">
+        <v>382</v>
+      </c>
+      <c r="E66" s="24">
+        <v>392</v>
+      </c>
+      <c r="F66" s="24">
+        <v>387</v>
+      </c>
+      <c r="G66" s="25">
+        <v>387</v>
+      </c>
+      <c r="H66" t="s">
+        <v>113</v>
+      </c>
+      <c r="I66" s="24"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A67" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="B67" s="24">
+        <v>60002</v>
+      </c>
+      <c r="C67">
+        <v>60</v>
+      </c>
+      <c r="D67" s="24">
+        <v>382</v>
+      </c>
+      <c r="E67" s="24">
+        <v>392</v>
+      </c>
+      <c r="F67" s="24">
+        <v>387</v>
+      </c>
+      <c r="G67" s="25">
+        <v>387</v>
+      </c>
+      <c r="H67" t="s">
+        <v>113</v>
+      </c>
+      <c r="I67" s="24"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A68" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="B68" s="24">
+        <v>60008</v>
+      </c>
+      <c r="C68">
+        <v>8</v>
+      </c>
+      <c r="D68" s="24">
+        <v>483</v>
+      </c>
+      <c r="E68" s="24">
+        <v>498</v>
+      </c>
+      <c r="F68" s="24">
+        <v>488</v>
+      </c>
+      <c r="G68" s="25">
+        <v>493</v>
+      </c>
+      <c r="H68" t="s">
+        <v>113</v>
+      </c>
+      <c r="I68" s="24"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A69" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="B69" s="24">
+        <v>60008</v>
+      </c>
+      <c r="C69">
+        <v>60</v>
+      </c>
+      <c r="D69" s="24">
+        <v>483</v>
+      </c>
+      <c r="E69" s="24">
+        <v>498</v>
+      </c>
+      <c r="F69" s="24">
+        <v>488</v>
+      </c>
+      <c r="G69" s="25">
+        <v>493</v>
+      </c>
+      <c r="H69" t="s">
+        <v>113</v>
+      </c>
+      <c r="I69" s="24"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A70" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="B70" s="24">
+        <v>70007</v>
+      </c>
+      <c r="C70">
+        <v>7</v>
+      </c>
+      <c r="D70" s="24">
+        <v>304</v>
+      </c>
+      <c r="E70" s="24">
+        <v>315</v>
+      </c>
+      <c r="F70" s="24">
+        <v>307</v>
+      </c>
+      <c r="G70" s="25">
+        <v>310</v>
+      </c>
+      <c r="H70" t="s">
+        <v>114</v>
+      </c>
+      <c r="I70" s="24"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A71" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="B71" s="24">
+        <v>70007</v>
+      </c>
+      <c r="C71">
+        <v>70</v>
+      </c>
+      <c r="D71" s="24">
+        <v>304</v>
+      </c>
+      <c r="E71" s="24">
+        <v>315</v>
+      </c>
+      <c r="F71" s="24">
+        <v>307</v>
+      </c>
+      <c r="G71" s="25">
+        <v>310</v>
+      </c>
+      <c r="H71" t="s">
+        <v>114</v>
+      </c>
+      <c r="I71" s="24"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A72" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="B72" s="24">
+        <v>70065</v>
+      </c>
+      <c r="C72">
+        <v>65</v>
+      </c>
+      <c r="D72" s="24">
+        <v>312</v>
+      </c>
+      <c r="E72" s="24">
+        <v>333</v>
+      </c>
+      <c r="F72" s="24">
+        <v>317</v>
+      </c>
+      <c r="G72" s="25">
+        <v>328</v>
+      </c>
+      <c r="H72" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="I72" s="24"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A73" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="B73" s="24">
+        <v>70065</v>
+      </c>
+      <c r="C73">
+        <v>70</v>
+      </c>
+      <c r="D73" s="24">
+        <v>312</v>
+      </c>
+      <c r="E73" s="24">
+        <v>333</v>
+      </c>
+      <c r="F73" s="24">
+        <v>317</v>
+      </c>
+      <c r="G73" s="25">
+        <v>328</v>
+      </c>
+      <c r="H73" t="s">
+        <v>114</v>
+      </c>
+      <c r="I73" s="24"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A74" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="B74" s="24">
+        <v>70069</v>
+      </c>
+      <c r="C74">
+        <v>69</v>
+      </c>
+      <c r="D74" s="24">
+        <v>373</v>
+      </c>
+      <c r="E74" s="24">
+        <v>391</v>
+      </c>
+      <c r="F74" s="24">
+        <v>378</v>
+      </c>
+      <c r="G74" s="25">
+        <v>386</v>
+      </c>
+      <c r="H74" t="s">
+        <v>114</v>
+      </c>
+      <c r="I74" s="24"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A75" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="B75" s="24">
+        <v>70069</v>
+      </c>
+      <c r="C75">
+        <v>70</v>
+      </c>
+      <c r="D75" s="24">
+        <v>373</v>
+      </c>
+      <c r="E75" s="24">
+        <v>391</v>
+      </c>
+      <c r="F75" s="24">
+        <v>378</v>
+      </c>
+      <c r="G75" s="25">
+        <v>386</v>
+      </c>
+      <c r="H75" t="s">
+        <v>114</v>
+      </c>
+      <c r="I75" s="24"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A76" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="B76" s="24">
+        <v>77069</v>
+      </c>
+      <c r="C76">
+        <v>69</v>
+      </c>
+      <c r="D76" s="24">
+        <v>389</v>
+      </c>
+      <c r="E76" s="24">
+        <v>407</v>
+      </c>
+      <c r="F76" s="24">
+        <v>394</v>
+      </c>
+      <c r="G76" s="25">
+        <v>402</v>
+      </c>
+      <c r="H76" t="s">
+        <v>114</v>
+      </c>
+      <c r="I76" s="24"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A77" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="B77" s="24">
+        <v>77069</v>
+      </c>
+      <c r="C77">
+        <v>77</v>
+      </c>
+      <c r="D77" s="24">
+        <v>389</v>
+      </c>
+      <c r="E77" s="24">
+        <v>407</v>
+      </c>
+      <c r="F77" s="24">
+        <v>394</v>
+      </c>
+      <c r="G77" s="25">
+        <v>402</v>
+      </c>
+      <c r="H77" t="s">
+        <v>114</v>
+      </c>
+      <c r="I77" s="24"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A78" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="B78" s="24">
+        <v>77070</v>
+      </c>
+      <c r="C78">
+        <v>70</v>
+      </c>
+      <c r="D78" s="24">
+        <v>414</v>
+      </c>
+      <c r="E78" s="24">
+        <v>432</v>
+      </c>
+      <c r="F78" s="24">
+        <v>419</v>
+      </c>
+      <c r="G78" s="25">
+        <v>427</v>
+      </c>
+      <c r="H78" t="s">
+        <v>113</v>
+      </c>
+      <c r="I78" s="24"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A79" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="B79" s="24">
+        <v>77070</v>
+      </c>
+      <c r="C79">
+        <v>70</v>
+      </c>
+      <c r="D79" s="24">
+        <v>414</v>
+      </c>
+      <c r="E79" s="24">
+        <v>432</v>
+      </c>
+      <c r="F79" s="24">
+        <v>419</v>
+      </c>
+      <c r="G79" s="25">
+        <v>427</v>
+      </c>
+      <c r="H79" t="s">
+        <v>113</v>
+      </c>
+      <c r="I79" s="24"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A80" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="B80" s="24">
+        <v>84083</v>
+      </c>
+      <c r="C80">
+        <v>83</v>
+      </c>
+      <c r="D80" s="24">
+        <v>421</v>
+      </c>
+      <c r="E80" s="24">
+        <v>432</v>
+      </c>
+      <c r="F80" s="24">
+        <v>426</v>
+      </c>
+      <c r="G80" s="25">
+        <v>427</v>
+      </c>
+      <c r="H80" t="s">
+        <v>113</v>
+      </c>
+      <c r="I80" s="24"/>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A81" s="23"/>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A82" s="23"/>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83" s="23"/>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A84" s="23"/>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A85" s="23"/>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A86" s="23"/>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A87" s="23"/>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A88" s="23"/>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A89" s="23"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="H39:H80">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="no">
+      <formula>NOT(ISERROR(SEARCH("no",H39)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="yes">
+      <formula>NOT(ISERROR(SEARCH("yes",H39)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="A14" sqref="A14:F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -1693,7 +3201,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>26</v>
       </c>
@@ -1726,7 +3234,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>27</v>
       </c>
@@ -1759,7 +3267,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>28</v>
       </c>
@@ -1792,7 +3300,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>29</v>
       </c>
@@ -1825,7 +3333,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>30</v>
       </c>
@@ -1858,7 +3366,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>31</v>
       </c>
@@ -1891,7 +3399,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>32</v>
       </c>
@@ -1924,7 +3432,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>33</v>
       </c>
@@ -1957,7 +3465,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>34</v>
       </c>
@@ -1990,7 +3498,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>35</v>
       </c>
@@ -2023,7 +3531,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>36</v>
       </c>
@@ -2056,7 +3564,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>39</v>
       </c>
@@ -2089,7 +3597,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>40</v>
       </c>
@@ -2122,7 +3630,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>41</v>
       </c>
@@ -2155,7 +3663,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>42</v>
       </c>
@@ -2188,7 +3696,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>43</v>
       </c>
@@ -2221,7 +3729,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>48</v>
       </c>
@@ -2254,7 +3762,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="str">
         <f>'clump-related'!A19</f>
         <v>macros3-1</v>
@@ -2290,7 +3798,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="str">
         <f>'clump-related'!A20</f>
         <v>macros3-2</v>
@@ -2326,7 +3834,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="str">
         <f>'clump-related'!A21</f>
         <v>macros3-3</v>
@@ -2362,7 +3870,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="str">
         <f>'clump-related'!A22</f>
         <v>macros3-4</v>
@@ -2398,7 +3906,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="str">
         <f>'clump-related'!A23</f>
         <v>macros3-5</v>
@@ -2434,7 +3942,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="str">
         <f>'clump-related'!A24</f>
         <v>macros3-6</v>
@@ -2470,7 +3978,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="str">
         <f>'clump-related'!A25</f>
         <v>macros3-7</v>
@@ -2506,7 +4014,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="str">
         <f>'clump-related'!A26</f>
         <v>macros3-8</v>
@@ -2542,7 +4050,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="str">
         <f>'clump-related'!A27</f>
         <v>macros3-9</v>
@@ -2578,7 +4086,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="str">
         <f>'clump-related'!A28</f>
         <v>macros3-10</v>
@@ -2614,7 +4122,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="str">
         <f>'clump-related'!A29</f>
         <v>macros3-11</v>
@@ -2650,7 +4158,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="str">
         <f>'clump-related'!A30</f>
         <v>macros3-12</v>
@@ -2686,7 +4194,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="str">
         <f>'clump-related'!A31</f>
         <v>macros3-13</v>
@@ -2722,7 +4230,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="str">
         <f>'clump-related'!A32</f>
         <v>macros3-14</v>
@@ -2758,7 +4266,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="str">
         <f>'clump-related'!A33</f>
         <v>macros3-15</v>
@@ -2794,7 +4302,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="str">
         <f>'clump-related'!A34</f>
         <v>macros3-16</v>
@@ -2830,7 +4338,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="str">
         <f>'clump-related'!A35</f>
         <v>macros3-17</v>
@@ -2866,7 +4374,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="str">
         <f>'clump-related'!A36</f>
         <v>macros3-18</v>
@@ -2902,7 +4410,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="str">
         <f>'clump-related'!A37</f>
         <v>macros3-19</v>
@@ -2938,7 +4446,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="str">
         <f>'clump-related'!A38</f>
         <v>macros3-20</v>
@@ -2974,7 +4482,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -2991,23 +4499,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView topLeftCell="A13" zoomScale="101" workbookViewId="0">
       <selection activeCell="B33" sqref="B33:E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3030,7 +4538,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -3047,7 +4555,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -3064,7 +4572,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -3081,7 +4589,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -3098,7 +4606,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -3115,7 +4623,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -3132,7 +4640,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -3149,7 +4657,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -3166,7 +4674,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -3183,7 +4691,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -3200,7 +4708,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -3217,7 +4725,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -3234,7 +4742,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -3251,7 +4759,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -3268,7 +4776,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -3285,7 +4793,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -3302,7 +4810,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -3319,7 +4827,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -3336,7 +4844,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -3353,7 +4861,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -3370,7 +4878,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -3387,7 +4895,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -3404,7 +4912,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>16</v>
       </c>
@@ -3421,7 +4929,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>17</v>
       </c>
@@ -3438,7 +4946,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>18</v>
       </c>
@@ -3455,7 +4963,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>19</v>
       </c>
@@ -3472,7 +4980,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>20</v>
       </c>
@@ -3489,7 +4997,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>21</v>
       </c>
@@ -3506,7 +5014,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>22</v>
       </c>
@@ -3523,7 +5031,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>23</v>
       </c>
@@ -3540,7 +5048,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>24</v>
       </c>
@@ -3557,7 +5065,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>25</v>
       </c>

</xml_diff>